<commit_message>
fix: teste.xlsx info error
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -26,17 +26,6 @@
   </si>
   <si>
     <t>Name 1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>pablo.o.polvo@gmail.com</t>
-    </r>
   </si>
   <si>
     <t>Here is your personal information:</t>
@@ -64,7 +53,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -82,12 +71,6 @@
     </font>
     <font>
       <b val="1"/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <u val="single"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -114,12 +97,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -140,6 +123,19 @@
       <bottom style="thin">
         <color indexed="11"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -192,6 +188,17 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
@@ -234,14 +241,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -252,33 +259,44 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -286,23 +304,34 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -312,7 +341,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -322,40 +351,52 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -378,9 +419,9 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1442,7 +1483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1451,7 +1492,8 @@
     <col min="1" max="1" width="18" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.3516" style="1" customWidth="1"/>
     <col min="3" max="4" width="18" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.85" customHeight="1">
@@ -1467,91 +1509,103 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="27.85" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="4">
         <v>4</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="D2" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" ht="27.6" customHeight="1">
+      <c r="A3" t="s" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" ht="27.6" customHeight="1">
-      <c r="A3" t="s" s="6">
+      <c r="B3" t="s" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s" s="10">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s" s="10">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="7">
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" ht="27.6" customHeight="1">
+      <c r="A4" t="s" s="8">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s" s="10">
         <v>5</v>
       </c>
-      <c r="C3" t="s" s="8">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" ht="27.6" customHeight="1">
-      <c r="A4" t="s" s="6">
+      <c r="D4" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="B4" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s" s="8">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s" s="8">
-        <v>11</v>
-      </c>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="14.7" customHeight="1" hidden="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
     </row>
     <row r="6" ht="14.7" customHeight="1" hidden="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="14"/>
     </row>
     <row r="7" ht="14.7" customHeight="1" hidden="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="14"/>
     </row>
     <row r="8" ht="14.7" customHeight="1" hidden="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" ht="14.7" customHeight="1" hidden="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" ht="14.7" customHeight="1" hidden="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" ht="14.7" customHeight="1">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="18"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="" tooltip="" display="pablo.o.polvo@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId2" location="" tooltip="" display="pablo.o.polvo@gmail.com"/>
-    <hyperlink ref="B4" r:id="rId3" location="" tooltip="" display="pablo.o.polvo@gmail.com"/>
-  </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>